<commit_message>
adding another LM dl2v to lm_coll_subset_170331
</commit_message>
<xml_diff>
--- a/geometry_analysis/data/PNcountsPerGlom.xlsx
+++ b/geometry_analysis/data/PNcountsPerGlom.xlsx
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -934,11 +934,11 @@
         <v>0.5</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="2"/>
     </row>

</xml_diff>